<commit_message>
can export unformatted excel file now
</commit_message>
<xml_diff>
--- a/WordAndExcelModels/Untitled.xlsx
+++ b/WordAndExcelModels/Untitled.xlsx
@@ -372,7 +372,817 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ĺ2"/>
-  <sheetData/>
+  <dimension ref="A1:U13"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>工单编号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>来电时间</v>
+      </c>
+      <c r="C1" t="str">
+        <v>热线号码</v>
+      </c>
+      <c r="D1" t="str">
+        <v>受理单位</v>
+      </c>
+      <c r="E1" t="str">
+        <v>来电人</v>
+      </c>
+      <c r="F1" t="str">
+        <v>来电号码</v>
+      </c>
+      <c r="G1" t="str">
+        <v>联系方式</v>
+      </c>
+      <c r="H1" t="str">
+        <v>来电人地址</v>
+      </c>
+      <c r="I1" t="str">
+        <v>问题分类</v>
+      </c>
+      <c r="J1" t="str">
+        <v>工单分类</v>
+      </c>
+      <c r="K1" t="str">
+        <v>发生地址</v>
+      </c>
+      <c r="L1" t="str">
+        <v>被反映单位</v>
+      </c>
+      <c r="M1" t="str">
+        <v>标题</v>
+      </c>
+      <c r="N1" t="str">
+        <v>主要内容</v>
+      </c>
+      <c r="O1" t="str">
+        <v>派单人员</v>
+      </c>
+      <c r="P1" t="str">
+        <v>派单时间</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>处理意见</v>
+      </c>
+      <c r="R1" t="str">
+        <v>截止时间</v>
+      </c>
+      <c r="S1" t="str">
+        <v>处理时限</v>
+      </c>
+      <c r="T1" t="str">
+        <v>承办单位</v>
+      </c>
+      <c r="U1" t="str">
+        <v>处理情况</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>电[2019]A-39415931</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2019-03-19 15:39:05</v>
+      </c>
+      <c r="C2" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D2" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E2" t="str">
+        <v>张先生</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1381188496</v>
+      </c>
+      <c r="G2" t="str">
+        <v xml:space="preserve"> 电话:13811837132</v>
+      </c>
+      <c r="H2" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I2" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="J2" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K2" t="str">
+        <v>不详</v>
+      </c>
+      <c r="L2" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M2" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="N2" t="str">
+        <v>市民反映，自己之前在易道用车网约车平台有过消费，消费后要求平台开发票，客服答复因为税务系统改造升级，市民询问是否是国家税务系统，客服说是，市民表示自己在其他平台消费为何都可以开，客服告知会尽快恢复，市民不认可，易道用车隶属于北京东方车云信息技术有限公司（公司在北京注册，具体注册信息查询不到），来电反映易道用车不开发票的问题。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O2" t="str">
+        <v>燕璐斌</v>
+      </c>
+      <c r="P2" t="str">
+        <v>2019-03-19 16:57:07</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>2019年3月19日16:56分16019号派单至市地税局分中心</v>
+      </c>
+      <c r="R2" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S2" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T2" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>电[2019]A-39515539</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2019-03-19 15:51:02</v>
+      </c>
+      <c r="C3" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D3" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E3" t="str">
+        <v>张先生</v>
+      </c>
+      <c r="F3" t="str">
+        <v>13910184444</v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve"> 电话:13910185744</v>
+      </c>
+      <c r="H3" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I3" t="str">
+        <v>税收减免优惠</v>
+      </c>
+      <c r="J3" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K3" t="str">
+        <v>不详</v>
+      </c>
+      <c r="L3" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M3" t="str">
+        <v>税务政策不合理</v>
+      </c>
+      <c r="N3" t="str">
+        <v>市民反映，北京市发出了三项扣税减免政策，但是自己三项扣税减免之后扣税额变成了0，咨询税务热线12366之后称变成0之后影响买房，不能补缴或者调整，这个政策是有问题，让进行三项扣税减免，执行了之后又影响买房，来电反映税务政策不合理问题。请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O3" t="str">
+        <v>王晗</v>
+      </c>
+      <c r="P3" t="str">
+        <v>2019-03-19 16:44:39</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>2019年3月19日11827号16:44分派单市地税局分中心</v>
+      </c>
+      <c r="R3" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S3" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T3" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>电[2019]A-39488033</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2019-03-19 14:55:08</v>
+      </c>
+      <c r="C4" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D4" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E4" t="str">
+        <v>李先生</v>
+      </c>
+      <c r="F4" t="str">
+        <v>13910093936</v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> 电话:13910098282</v>
+      </c>
+      <c r="H4" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I4" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="J4" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K4" t="str">
+        <v>巴沟地铁站西侧紧邻处华联超市</v>
+      </c>
+      <c r="L4" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M4" t="str">
+        <v>华联超市物业不开发票“12350热线来电”</v>
+      </c>
+      <c r="N4" t="str">
+        <v>市民反映，自己在海淀区海淀街道（网络查询）巴沟地铁站西侧紧邻处华联超市租赁店面，物业名称：北京华联万贸购物中心金银有限公司，市民称自己店名：麦趣尔，装修时多次被物业罚款，多次索要发票均不提供，导致市民无法报账，时间：2019年2月底，罚款项目：施工罚款，金额：1万元、2000多元共两次，来电反映华联超市物业不开发票的问题。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O4" t="str">
+        <v>王志博</v>
+      </c>
+      <c r="P4" t="str">
+        <v>2019-03-19 16:43:32</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>2019年3月19日15779号16:43分针对诉求点派单市地税局分中心</v>
+      </c>
+      <c r="R4" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S4" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T4" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>电[2019]A-39543342</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2019-03-19 09:41:04</v>
+      </c>
+      <c r="C5" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D5" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E5" t="str">
+        <v>胡女士</v>
+      </c>
+      <c r="F5" t="str">
+        <v>13562142093</v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> 电话:13501342093</v>
+      </c>
+      <c r="H5" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I5" t="str">
+        <v>税（费）种征收</v>
+      </c>
+      <c r="J5" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K5" t="str">
+        <v>西城行政服务大厅</v>
+      </c>
+      <c r="L5" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M5" t="str">
+        <v>映税务局迟迟没有回复</v>
+      </c>
+      <c r="N5" t="str">
+        <v>市民反映，自己注销的的营业执照的北京中苑金典科技有限公司，自己在3月6号办的注销已经把所有税补完了，在西城行政服务大厅，说3到5天，但是现在还没有给自己反馈，法人：胡军华，税号：110104667516769，来电反映税务局迟迟没有回复的问题。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O5" t="str">
+        <v>齐茹</v>
+      </c>
+      <c r="P5" t="str">
+        <v>2019-03-19 16:42:19</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>2019年3月19日15521号16:42分针对问题派单至市地税局。</v>
+      </c>
+      <c r="R5" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S5" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T5" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>电[2019]A-54135923</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2019-03-19 15:05:31</v>
+      </c>
+      <c r="C6" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D6" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E6" t="str">
+        <v>朴女士</v>
+      </c>
+      <c r="F6" t="str">
+        <v>13010615197</v>
+      </c>
+      <c r="G6" t="str">
+        <v xml:space="preserve"> 电话:18810515197</v>
+      </c>
+      <c r="H6" t="str">
+        <v>中国北京市朝阳区</v>
+      </c>
+      <c r="I6" t="str">
+        <v>税（费）种征收</v>
+      </c>
+      <c r="J6" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K6" t="str">
+        <v>回族乡人民政府</v>
+      </c>
+      <c r="L6" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M6" t="str">
+        <v>不给销发票</v>
+      </c>
+      <c r="N6" t="str">
+        <v>市民反映，自己3月13日在朝阳区常营乡回族乡人民政府开的个人租赁发票，由于自己开的发票开错了，想把发票销了，然后重开，他们说没有那个权限，自己到了世通大厦税务局咨询了，他们说哪开的在哪销，别的地方也销不了，地址：朝阳区常营乡回族乡人民政府，来电反映不给销发票的问题。注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O6" t="str">
+        <v>陈鑫</v>
+      </c>
+      <c r="P6" t="str">
+        <v>2019-03-19 15:41:50</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>2019年3月19日15：40分14049号针对问题派单市地税局分中心</v>
+      </c>
+      <c r="R6" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S6" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T6" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>电[2019]A-39562042</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2019-03-19 15:22:39</v>
+      </c>
+      <c r="C7" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D7" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E7" t="str">
+        <v>卢女士</v>
+      </c>
+      <c r="F7" t="str">
+        <v>13581956378</v>
+      </c>
+      <c r="G7" t="str">
+        <v xml:space="preserve"> 电话:13581988387</v>
+      </c>
+      <c r="H7" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I7" t="str">
+        <v>管理服务不规范</v>
+      </c>
+      <c r="J7" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K7" t="str">
+        <v>华远街19号置地星座地下停车场</v>
+      </c>
+      <c r="L7" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M7" t="str">
+        <v>停车场收费不给开发票问题”12319热线来电“</v>
+      </c>
+      <c r="N7" t="str">
+        <v xml:space="preserve">市民反映，3月16日晚上9:50分在西城区华远街19号置地星座地下停车场内停车，一共花了19.5元钱，自己是基本每周都会到停车场，上周自己就的时候，收费人员说可以微信支付了，自己支付了之后对方就给自己开了一张票，这次自己通过微信支付之后要求对方提供发票，对方就不给提供，说是停车场是ETCP标识，自己说上一次就给票了，后来这个人就说上次不是他值班的，自己打了晚上商场值班的电话，去了两个人态度强硬的，还是不给开发票，来电希望相关部门帮助核实停车场收费不给开发票问题。 注：请及时向来电人反馈办理情况。 </v>
+      </c>
+      <c r="O7" t="str">
+        <v>张立静</v>
+      </c>
+      <c r="P7" t="str">
+        <v>2019-03-19 15:39:01</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>2019年3月19日15：38分16502号针对问题派单至市国家税务局。</v>
+      </c>
+      <c r="R7" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S7" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T7" t="str">
+        <v>市国家税务局</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>电[2019]A-54233014</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2019-03-19 13:03:43</v>
+      </c>
+      <c r="C8" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D8" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E8" t="str">
+        <v>司先生</v>
+      </c>
+      <c r="F8" t="str">
+        <v>18513349999</v>
+      </c>
+      <c r="G8" t="str">
+        <v xml:space="preserve"> 电话:18513343599</v>
+      </c>
+      <c r="H8" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I8" t="str">
+        <v>偷逃税款</v>
+      </c>
+      <c r="J8" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K8" t="str">
+        <v>西罗园北路河南商务会馆</v>
+      </c>
+      <c r="L8" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M8" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="N8" t="str">
+        <v>市民反映，2018年12月12日晚上9点中丰台区西罗园街道西罗园北路河南商务会馆吃饭，当时花费371元，因为吃完饭已经到晚上10点多了，当时饭店已经下班了，饭店给市民承诺留有小票随时可以来开发票，2019年3月19日找到该店开具发票，但是店家称税务规定超过一个月就不可以开发票了，并且已经跨年了，更不可以开具，来电反映不开发票的问题。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O8" t="str">
+        <v>王春雨</v>
+      </c>
+      <c r="P8" t="str">
+        <v>2019-03-19 15:36:03</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>2019年3月19日15:35分11844号派单市国家税务局。</v>
+      </c>
+      <c r="R8" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S8" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T8" t="str">
+        <v>市国家税务局</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>电[2019]A-54193509</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2019-03-19 14:32:11</v>
+      </c>
+      <c r="C9" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D9" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E9" t="str">
+        <v>朴先生</v>
+      </c>
+      <c r="F9" t="str">
+        <v>017110000019</v>
+      </c>
+      <c r="G9" t="str">
+        <v xml:space="preserve"> 电话:017110180019</v>
+      </c>
+      <c r="H9" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I9" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="J9" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K9" t="str">
+        <v>港旅大厦B1层</v>
+      </c>
+      <c r="L9" t="str">
+        <v>望京小腰</v>
+      </c>
+      <c r="M9" t="str">
+        <v>望京小腰不开发票</v>
+      </c>
+      <c r="N9" t="str">
+        <v>市民反映，4、5天之前在朝阳区望京街道港旅大厦B1层望京小腰吃饭，消费400多元，要求对方开发票，但是对方说没有发票，来电希望相关部门核实处理不开发票问题。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O9" t="str">
+        <v>齐茹</v>
+      </c>
+      <c r="P9" t="str">
+        <v>2019-03-19 15:25:23</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>2019年3月19日15521号15:25分针对问题派单至市地税局。</v>
+      </c>
+      <c r="R9" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S9" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T9" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>电[2019]A-39612936</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2019-03-19 12:57:30</v>
+      </c>
+      <c r="C10" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D10" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E10" t="str">
+        <v>王先生</v>
+      </c>
+      <c r="F10" t="str">
+        <v>13811945536</v>
+      </c>
+      <c r="G10" t="str">
+        <v xml:space="preserve"> 电话:13811810536</v>
+      </c>
+      <c r="H10" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I10" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="J10" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K10" t="str">
+        <v>老巷子家常菜</v>
+      </c>
+      <c r="L10" t="str">
+        <v>老巷子家常菜</v>
+      </c>
+      <c r="M10" t="str">
+        <v>老巷子家常菜商家未开发票</v>
+      </c>
+      <c r="N10" t="str">
+        <v>市民反映，在通州区宋庄镇老巷子家常菜，自己经常在这吃饭，没有提供发票，店家总是推脱，在2019年3月19日12点在这吃饭，自己还拿着前两天3月14号中午的时候在这吃饭未开发票的单子去找商家要发票，商家依旧推脱，已经好几次了，来电反映老巷子家常菜商家未开发票问题。 注：手机号：13716672054。 注：请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O10" t="str">
+        <v>魏玉婷</v>
+      </c>
+      <c r="P10" t="str">
+        <v>2019-03-19 14:53:58</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>2019年3月19日14:53分16011号针对市民诉求派单至市地税局分中心</v>
+      </c>
+      <c r="R10" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S10" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T10" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>电[2019]A-54115023</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2019-03-19 09:10:19</v>
+      </c>
+      <c r="C11" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D11" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E11" t="str">
+        <v>EMPTY</v>
+      </c>
+      <c r="F11" t="str">
+        <v>13011840840</v>
+      </c>
+      <c r="G11" t="str">
+        <v>EMPTY</v>
+      </c>
+      <c r="H11" t="str">
+        <v>EMPTY</v>
+      </c>
+      <c r="I11" t="str">
+        <v>偷逃税款</v>
+      </c>
+      <c r="J11" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K11" t="str">
+        <v>北京经济技术开发区荣华中路7号院2号楼18层1806</v>
+      </c>
+      <c r="L11" t="str">
+        <v>EMPTY</v>
+      </c>
+      <c r="M11" t="str">
+        <v>偷税漏税问题</v>
+      </c>
+      <c r="N11" t="str">
+        <v>市民反映，自己2019年1月10号左右入职，2月多离职，和公司没有签合同，发现公司的收入都是通过个人的账户，不通过公户结算，不缴纳税款，存在偷税漏税，希望有关部门调查处理，公司：北京千外家亦博房地产经济有限公司，注册地址：北京市北京经济技术开发区荣华中路7号院2号楼18层1806，办公地址：昌平区回龙观镇北京人家1号楼底商，来电希望相关部门帮助解决偷税漏税问题。注：请及时向反映人反馈办理信息</v>
+      </c>
+      <c r="O11" t="str">
+        <v>王猛2</v>
+      </c>
+      <c r="P11" t="str">
+        <v>2019-03-19 14:31:35</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>2019年3月19日11824号14:31分针对上述问题派单市国家税务局。</v>
+      </c>
+      <c r="R11" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S11" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T11" t="str">
+        <v>市国家税务局</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>电[2019]A-39491932</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2019-03-19 12:09:45</v>
+      </c>
+      <c r="C12" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D12" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E12" t="str">
+        <v>刘女士</v>
+      </c>
+      <c r="F12" t="str">
+        <v>13880020880</v>
+      </c>
+      <c r="G12" t="str">
+        <v xml:space="preserve"> 电话:13426020880</v>
+      </c>
+      <c r="H12" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I12" t="str">
+        <v>不开发票</v>
+      </c>
+      <c r="J12" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K12" t="str">
+        <v>新世界商场地下一层新世界超市</v>
+      </c>
+      <c r="L12" t="str">
+        <v>新世界超市</v>
+      </c>
+      <c r="M12" t="str">
+        <v>超市不给开发票</v>
+      </c>
+      <c r="N12" t="str">
+        <v>市民反映，自己在东城区崇文门外街道新世界商场地下一层的新世界超市，要求开具发票，但是超市不给开，市民手里持有攒了一个月的超市购物小票，但是超市工作人员称，自2019年1月1日超市开发票的相关规定改为，还需要市民每一笔消费使用的微信、支付宝、银行卡的消费凭据，才可以开发票，市民认为不合理。来电反映超市不给开发票的问题。请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O12" t="str">
+        <v>王晗</v>
+      </c>
+      <c r="P12" t="str">
+        <v>2019-03-19 14:29:42</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>2019年3月19日11827号14:27分派单市地税局分中心</v>
+      </c>
+      <c r="R12" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S12" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T12" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>电[2019]A-54191515</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2019-03-19 13:04:52</v>
+      </c>
+      <c r="C13" t="str">
+        <v>12345</v>
+      </c>
+      <c r="D13" t="str">
+        <v>北京市非紧急救助服务中心</v>
+      </c>
+      <c r="E13" t="str">
+        <v>周先生</v>
+      </c>
+      <c r="F13" t="str">
+        <v>18852565888</v>
+      </c>
+      <c r="G13" t="str">
+        <v xml:space="preserve"> 电话:18910565888</v>
+      </c>
+      <c r="H13" t="str">
+        <v>中国北京市</v>
+      </c>
+      <c r="I13" t="str">
+        <v>发票造假</v>
+      </c>
+      <c r="J13" t="str">
+        <v>诉求</v>
+      </c>
+      <c r="K13" t="str">
+        <v>大成路京客隆超市青塔店</v>
+      </c>
+      <c r="L13" t="str">
+        <v>不详</v>
+      </c>
+      <c r="M13" t="str">
+        <v>停车场定额发票不盖章</v>
+      </c>
+      <c r="N13" t="str">
+        <v>市民反映，自己在今天（3月19日12:00分左右）在丰台区卢沟桥街道大成路京客隆超市青塔店收费停车场停车，自己刚刚（2019年3月19日13:07分）出来，交完停车费，给了自己5元钱定额发票，发票上没有单位盖章，自己问了收费人员，收费人员说都是这样，车牌号：京Q96VR3,来电反映停车场定额发票不盖章的问题。  请及时向来电人反馈办理情况。</v>
+      </c>
+      <c r="O13" t="str">
+        <v>王晗</v>
+      </c>
+      <c r="P13" t="str">
+        <v>2019-03-19 14:28:06</v>
+      </c>
+      <c r="Q13" t="str">
+        <v>2019年3月19日11827号14:27分派单市地税局分中心</v>
+      </c>
+      <c r="R13" t="str">
+        <v>2019-04-10 23:59:59</v>
+      </c>
+      <c r="S13" t="str">
+        <v>15工作日</v>
+      </c>
+      <c r="T13" t="str">
+        <v>市地税局分中心</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add outerNetworkNumber into feedbackContent
</commit_message>
<xml_diff>
--- a/WordAndExcelModels/Untitled.xlsx
+++ b/WordAndExcelModels/Untitled.xlsx
@@ -465,11 +465,11 @@
         <v>11</v>
       </c>
       <c r="L2" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39415931
+        <v xml:space="preserve">外网编号：201939415931
 来点人姓名：张先生
 联系电话：1381188496
 主要内容：不开发票
-反映内容：-</v>
+反映内容：5</v>
       </c>
       <c r="M2" t="str">
         <v>见举报内容</v>
@@ -525,11 +525,11 @@
         <v>11</v>
       </c>
       <c r="L3" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39515539
+        <v xml:space="preserve">外网编号：201939515539
 来点人姓名：张先生
 联系电话：13910184444
 主要内容：税务政策不合理
-反映内容：-</v>
+反映内容：5</v>
       </c>
       <c r="M3" t="str">
         <v>见举报内容</v>
@@ -585,11 +585,11 @@
         <v>11</v>
       </c>
       <c r="L4" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39488033
+        <v xml:space="preserve">外网编号：201939488033
 来点人姓名：李先生
 联系电话：13910093936
 主要内容：华联超市物业不开发票“12350热线来电”
-反映内容：-</v>
+反映内容：8</v>
       </c>
       <c r="M4" t="str">
         <v>见举报内容</v>
@@ -645,11 +645,11 @@
         <v>11</v>
       </c>
       <c r="L5" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39543342
+        <v xml:space="preserve">外网编号：201939543342
 来点人姓名：胡女士
 联系电话：13562142093
 主要内容：映税务局迟迟没有回复
-反映内容：-</v>
+反映内容：3</v>
       </c>
       <c r="M5" t="str">
         <v>见举报内容</v>
@@ -705,11 +705,11 @@
         <v>11</v>
       </c>
       <c r="L6" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-54135923
+        <v xml:space="preserve">外网编号：201954135923
 来点人姓名：朴女士
 联系电话：13010615197
 主要内容：不给销发票
-反映内容：-</v>
+反映内容：5</v>
       </c>
       <c r="M6" t="str">
         <v>见举报内容</v>
@@ -765,11 +765,11 @@
         <v>11</v>
       </c>
       <c r="L7" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39562042
+        <v xml:space="preserve">外网编号：201939562042
 来点人姓名：卢女士
 联系电话：13581956378
 主要内容：停车场收费不给开发票问题”12319热线来电“
-反映内容：-</v>
+反映内容：2</v>
       </c>
       <c r="M7" t="str">
         <v>见举报内容</v>
@@ -825,11 +825,11 @@
         <v>11</v>
       </c>
       <c r="L8" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-54233014
+        <v xml:space="preserve">外网编号：201954233014
 来点人姓名：司先生
 联系电话：18513349999
 主要内容：不开发票
-反映内容：-</v>
+反映内容：3</v>
       </c>
       <c r="M8" t="str">
         <v>见举报内容</v>
@@ -885,11 +885,11 @@
         <v>11</v>
       </c>
       <c r="L9" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-54193509
+        <v xml:space="preserve">外网编号：201954193509
 来点人姓名：朴先生
 联系电话：017110000019
 主要内容：望京小腰不开发票
-反映内容：-</v>
+反映内容：3</v>
       </c>
       <c r="M9" t="str">
         <v>见举报内容</v>
@@ -945,11 +945,11 @@
         <v>11</v>
       </c>
       <c r="L10" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39612936
+        <v xml:space="preserve">外网编号：201939612936
 来点人姓名：王先生
 联系电话：13811945536
 主要内容：老巷子家常菜商家未开发票
-反映内容：-</v>
+反映内容：2</v>
       </c>
       <c r="M10" t="str">
         <v>见举报内容</v>
@@ -981,7 +981,7 @@
         <v>2019-03-19 14:31:35</v>
       </c>
       <c r="D11" t="str">
-        <v>EMPTY</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E11" t="str">
         <v xml:space="preserve"> </v>
@@ -1005,11 +1005,11 @@
         <v>11</v>
       </c>
       <c r="L11" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-54115023
-来点人姓名：EMPTY
+        <v xml:space="preserve">外网编号：201954115023
+来点人姓名： 
 联系电话：13011840840
 主要内容：偷税漏税问题
-反映内容：-</v>
+反映内容：5</v>
       </c>
       <c r="M11" t="str">
         <v>见举报内容</v>
@@ -1065,11 +1065,11 @@
         <v>11</v>
       </c>
       <c r="L12" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-39491932
+        <v xml:space="preserve">外网编号：201939491932
 来点人姓名：刘女士
 联系电话：13880020880
 主要内容：超市不给开发票
-反映内容：-</v>
+反映内容：1</v>
       </c>
       <c r="M12" t="str">
         <v>见举报内容</v>
@@ -1125,11 +1125,11 @@
         <v>11</v>
       </c>
       <c r="L13" t="str" xml:space="preserve">
-        <v xml:space="preserve">外网编号：电[2019]A-54191515
+        <v xml:space="preserve">外网编号：201954191515
 来点人姓名：周先生
 联系电话：18852565888
 主要内容：停车场定额发票不盖章
-反映内容：-</v>
+反映内容：1</v>
       </c>
       <c r="M13" t="str">
         <v>见举报内容</v>

</xml_diff>